<commit_message>
Updated requirements.txt to include missing req
</commit_message>
<xml_diff>
--- a/Scout_Config.xlsx
+++ b/Scout_Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephmonaghan/Documents/nanoDESI_raw_to_imzml/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://viucanada-my.sharepoint.com/personal/kyle_duncan_viu_ca/Documents/5_VIU/2_Research/2_Projects/Joseph M/imZML Writer/imzML_TechnicalNote/imzML_Writer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0F1E63-71CD-9740-AD8E-7B9C4EEA3C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{7A0F1E63-71CD-9740-AD8E-7B9C4EEA3C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C74A1664-4259-ED4D-8086-5F8B7D75C735}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{E678C7BB-EDE3-404C-BC63-8B37D1672C01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Cmap_Options</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>hot</t>
+  </si>
+  <si>
+    <t>Blues</t>
+  </si>
+  <si>
+    <t>Reds</t>
+  </si>
+  <si>
+    <t>Greens</t>
+  </si>
+  <si>
+    <t>Oranges</t>
   </si>
 </sst>
 </file>
@@ -422,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B39411C-266F-E44B-AAD5-9DB09F8077DB}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,6 +467,26 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>